<commit_message>
establish Soc Quicima operating model
</commit_message>
<xml_diff>
--- a/Industrials/Soc Quimica/Soc Quimica Valuation.xlsx
+++ b/Industrials/Soc Quimica/Soc Quimica Valuation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianyu/Desktop/Finance/Financial_Analysis/Industrials/Soc Quimica/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Finance\Financial_Analysis\Industrials\Soc Quimica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421398B5-BECC-A347-A070-81922E787532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D7F8B8-12C6-4F6B-B811-44ECEC0E1554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25720" windowHeight="18880" activeTab="2" xr2:uid="{CDED3339-8939-2C43-8CE7-BFDE9000B176}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CDED3339-8939-2C43-8CE7-BFDE9000B176}"/>
   </bookViews>
   <sheets>
     <sheet name="Public Comps" sheetId="2" r:id="rId1"/>
@@ -1932,6 +1932,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1995,8 +1997,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="ChartingText" xfId="20" xr:uid="{2F903AD7-622C-455A-B98A-ABBFF5B29CA1}"/>
@@ -3389,24 +3389,24 @@
     <v>Learn more on Bing</v>
   </rv>
   <rv s="3">
+    <v>en-US</v>
+    <v>a1mv7w</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
     <v>0</v>
     <v>ADOBE INC. (XNAS:ADBE)</v>
     <v>3</v>
     <v>4</v>
     <v>Finance</v>
     <v>5</v>
-    <v>en-US</v>
-    <v>a1mv7w</v>
-    <v>268435456</v>
-    <v>1</v>
-    <v>Powered by Refinitiv</v>
     <v>625.83410000000003</v>
     <v>318.60000000000002</v>
     <v>1.3439000000000001</v>
     <v>4.05</v>
+    <v>1.5079999999999998E-3</v>
     <v>6.5400000000000007E-3</v>
-    <v>-0.12</v>
-    <v>-1.9249999999999999E-4</v>
+    <v>0.94</v>
     <v>USD</v>
     <v>Adobe Inc. is a software company that offers a line of products and services used by professionals, communicators, businesses, and consumers for creating, managing, delivering, measuring, optimizing, engaging and transacting with content and experiences across various digital media formats. The Company’s segments include Digital Media, Digital Experience and Publishing and Advertising. Digital Media segment provides products, services and solutions that enable individuals, teams and enterprises to create, publish and promote their content anywhere. Digital Media segment is centered around Adobe Creative Cloud and Adobe Document Cloud. Digital Experience segment provides an integrated platform and set of applications and services through Adobe Experience Cloud that enable brands and businesses to create, manage, execute, measure, monetize and optimize customer experiences. The Publishing and Advertising segment consists of products and services that address diverse market opportunities.</v>
     <v>29239</v>
@@ -3418,7 +3418,7 @@
     <v>3</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45258.944064397656</v>
+    <v>45258.917360242966</v>
     <v>4</v>
     <v>612.26</v>
     <v>283797596000</v>
@@ -3428,11 +3428,11 @@
     <v>55.756500000000003</v>
     <v>619.27</v>
     <v>623.32000000000005</v>
-    <v>623.20000000000005</v>
+    <v>624.26</v>
     <v>455300000</v>
     <v>ADBE</v>
     <v>ADOBE INC. (XNAS:ADBE)</v>
-    <v>2302265</v>
+    <v>2302913</v>
     <v>2473701</v>
     <v>1997</v>
   </rv>
@@ -3461,24 +3461,24 @@
     <k n="Text" t="s"/>
   </s>
   <s t="_linkedentitycore">
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
     <k n="_Display" t="spb"/>
     <k n="_DisplayString" t="s"/>
     <k n="_Flags" t="spb"/>
     <k n="_Format" t="spb"/>
     <k n="_Icon" t="s"/>
     <k n="_SubLabel" t="spb"/>
-    <k n="%EntityCulture" t="s"/>
-    <k n="%EntityId" t="s"/>
-    <k n="%EntityServiceId"/>
-    <k n="%IsRefreshable" t="b"/>
-    <k n="%ProviderInfo" t="s"/>
     <k n="52 week high"/>
     <k n="52 week low"/>
     <k n="Beta"/>
     <k n="Change"/>
+    <k n="Change % (Extended hours)"/>
     <k n="Change (%)"/>
     <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -3618,9 +3618,9 @@
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
+      <v>Source: Nasdaq</v>
       <v>GMT</v>
-      <v>Real-Time Nasdaq Last Sale</v>
+      <v>Delayed 15 minutes</v>
       <v>from close</v>
       <v>from close</v>
     </spb>
@@ -3706,7 +3706,7 @@
       <x:numFmt numFmtId="0" formatCode="General"/>
     </x:dxf>
     <x:dxf>
-      <x:numFmt numFmtId="27" formatCode="m/d/yy\ h:mm"/>
+      <x:numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </x:dxf>
     <x:dxf>
       <x:numFmt numFmtId="14" formatCode="0.00%"/>
@@ -4062,20 +4062,20 @@
       <selection pane="topRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="35" customWidth="1"/>
+    <col min="1" max="1" width="62.296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.69921875" style="35" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.19921875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.19921875" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="14.69921875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="106" t="s">
         <v>207</v>
       </c>
@@ -4087,7 +4087,7 @@
       <c r="G2" s="51"/>
       <c r="H2" s="51"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>208</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C4" s="34"/>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
@@ -4121,7 +4121,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="160" t="s">
         <v>232</v>
       </c>
@@ -4133,7 +4133,7 @@
       <c r="G5" s="161"/>
       <c r="H5" s="161"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
       <c r="C6" s="154"/>
@@ -4143,7 +4143,7 @@
       <c r="G6" s="154"/>
       <c r="H6" s="154"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="170" t="s">
         <v>233</v>
       </c>
@@ -4157,11 +4157,11 @@
       <c r="G7" s="169"/>
       <c r="H7" s="169"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="170" t="s">
         <v>234</v>
       </c>
-      <c r="B8" s="197" t="s">
+      <c r="B8" s="199" t="s">
         <v>211</v>
       </c>
       <c r="C8" s="154"/>
@@ -4171,11 +4171,11 @@
       <c r="G8" s="154"/>
       <c r="H8" s="154"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="170" t="s">
         <v>235</v>
       </c>
-      <c r="B9" s="198"/>
+      <c r="B9" s="200"/>
       <c r="C9" s="154"/>
       <c r="D9" s="154"/>
       <c r="E9" s="154"/>
@@ -4183,11 +4183,11 @@
       <c r="G9" s="154"/>
       <c r="H9" s="154"/>
     </row>
-    <row r="10" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="170" t="s">
         <v>236</v>
       </c>
-      <c r="B10" s="199" t="s">
+      <c r="B10" s="201" t="s">
         <v>212</v>
       </c>
       <c r="C10" s="178"/>
@@ -4197,11 +4197,11 @@
       <c r="G10" s="178"/>
       <c r="H10" s="178"/>
     </row>
-    <row r="11" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="170" t="s">
         <v>237</v>
       </c>
-      <c r="B11" s="200"/>
+      <c r="B11" s="202"/>
       <c r="C11" s="154"/>
       <c r="D11" s="154"/>
       <c r="E11" s="154"/>
@@ -4209,11 +4209,11 @@
       <c r="G11" s="154"/>
       <c r="H11" s="154"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="170" t="s">
         <v>238</v>
       </c>
-      <c r="B12" s="201"/>
+      <c r="B12" s="203"/>
       <c r="C12" s="154"/>
       <c r="D12" s="154"/>
       <c r="E12" s="154"/>
@@ -4221,7 +4221,7 @@
       <c r="G12" s="154"/>
       <c r="H12" s="154"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="170" t="s">
         <v>239</v>
       </c>
@@ -4235,7 +4235,7 @@
       <c r="G13" s="169"/>
       <c r="H13" s="169"/>
     </row>
-    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="155"/>
@@ -4245,7 +4245,7 @@
       <c r="G14" s="155"/>
       <c r="H14" s="155"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>215</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>214</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>5</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>6</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="155"/>
       <c r="D21" s="155"/>
       <c r="E21" s="155"/>
@@ -4415,7 +4415,7 @@
       <c r="G21" s="155"/>
       <c r="H21" s="155"/>
     </row>
-    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>221</v>
       </c>
@@ -4439,14 +4439,14 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="174"/>
       <c r="C27" s="35"/>
       <c r="D27" s="35"/>
       <c r="E27" s="35"/>
       <c r="F27" s="35"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="163"/>
       <c r="C28" s="3"/>
@@ -4456,23 +4456,23 @@
       <c r="G28" s="33"/>
       <c r="H28" s="33"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="173"/>
-      <c r="C29" s="202"/>
+      <c r="C29" s="204"/>
       <c r="D29" s="173"/>
       <c r="E29" s="35"/>
       <c r="F29" s="35"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="173"/>
-      <c r="C30" s="203"/>
+      <c r="C30" s="205"/>
       <c r="D30" s="173"/>
       <c r="E30" s="35"/>
       <c r="F30" s="35"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="173"/>
-      <c r="C31" s="203"/>
+      <c r="C31" s="205"/>
       <c r="D31" s="173"/>
       <c r="E31" s="35"/>
       <c r="F31" s="35"/>
@@ -4497,33 +4497,33 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.69921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.69921875" style="1" customWidth="1"/>
     <col min="5" max="5" width="3" style="1" customWidth="1"/>
-    <col min="6" max="10" width="15.33203125" style="1" customWidth="1"/>
+    <col min="6" max="10" width="15.296875" style="1" customWidth="1"/>
     <col min="11" max="14" width="15.5" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.83203125" style="1"/>
-    <col min="17" max="17" width="9.6640625" style="1" customWidth="1"/>
-    <col min="18" max="36" width="10.83203125" style="1"/>
-    <col min="37" max="37" width="24.83203125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.796875" style="1"/>
+    <col min="17" max="17" width="9.69921875" style="1" customWidth="1"/>
+    <col min="18" max="36" width="10.796875" style="1"/>
+    <col min="37" max="37" width="24.796875" style="1" customWidth="1"/>
     <col min="38" max="38" width="16.5" style="1" customWidth="1"/>
-    <col min="39" max="39" width="25.1640625" style="1" customWidth="1"/>
-    <col min="40" max="41" width="10.1640625" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="10.83203125" style="1"/>
+    <col min="39" max="39" width="25.19921875" style="1" customWidth="1"/>
+    <col min="40" max="41" width="10.19921875" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="144" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
     </row>
-    <row r="3" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="110" t="s">
         <v>229</v>
       </c>
@@ -4541,12 +4541,12 @@
       <c r="M3" s="65"/>
       <c r="N3" s="66"/>
     </row>
-    <row r="4" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="205" t="s">
+    <row r="4" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="207" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="206"/>
-      <c r="D4" s="207"/>
+      <c r="C4" s="208"/>
+      <c r="D4" s="209"/>
       <c r="F4" s="67" t="s">
         <v>199</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="38" t="s">
         <v>10</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
         <v>219</v>
       </c>
@@ -4607,7 +4607,7 @@
       <c r="N6" s="72"/>
       <c r="O6" s="151"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="38" t="s">
         <v>220</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="38"/>
       <c r="D8" s="72"/>
       <c r="F8" s="38" t="s">
@@ -4667,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
         <v>15</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="38" t="s">
         <v>217</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="38"/>
       <c r="C11" s="90"/>
       <c r="D11" s="87"/>
@@ -4762,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="38" t="s">
         <v>216</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>1522921.6074508803</v>
       </c>
     </row>
-    <row r="13" spans="2:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="38" t="s">
         <v>19</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="38"/>
       <c r="D14" s="72"/>
       <c r="F14" s="81" t="s">
@@ -4857,7 +4857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="38" t="s">
         <v>21</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>1522921.6074508803</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
         <v>23</v>
       </c>
@@ -4926,7 +4926,7 @@
       <c r="P16" s="52"/>
       <c r="Q16" s="52"/>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:40" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="38" t="s">
         <v>25</v>
       </c>
@@ -4967,7 +4967,7 @@
       <c r="V17" s="54"/>
       <c r="W17" s="54"/>
     </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B18" s="38" t="s">
         <v>27</v>
       </c>
@@ -4976,15 +4976,15 @@
         <v>0.11299999999999999</v>
       </c>
       <c r="D18" s="72"/>
-      <c r="Q18" s="204"/>
-      <c r="R18" s="204"/>
-      <c r="S18" s="204"/>
-      <c r="T18" s="204"/>
-      <c r="U18" s="204"/>
-      <c r="V18" s="204"/>
-      <c r="W18" s="204"/>
-    </row>
-    <row r="19" spans="2:40" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q18" s="206"/>
+      <c r="R18" s="206"/>
+      <c r="S18" s="206"/>
+      <c r="T18" s="206"/>
+      <c r="U18" s="206"/>
+      <c r="V18" s="206"/>
+      <c r="W18" s="206"/>
+    </row>
+    <row r="19" spans="2:40" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="38"/>
       <c r="D19" s="72"/>
       <c r="F19" s="110" t="s">
@@ -5003,7 +5003,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B20" s="38" t="s">
         <v>30</v>
       </c>
@@ -5025,7 +5025,7 @@
         <f>Schedules!N24</f>
         <v>1522921.6074508803</v>
       </c>
-      <c r="P20" s="208" t="s">
+      <c r="P20" s="210" t="s">
         <v>34</v>
       </c>
       <c r="Q20" s="55">
@@ -5051,7 +5051,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B21" s="38"/>
       <c r="D21" s="72"/>
       <c r="F21" s="81" t="s">
@@ -5072,7 +5072,7 @@
         <f>C34</f>
         <v>21</v>
       </c>
-      <c r="P21" s="208"/>
+      <c r="P21" s="210"/>
       <c r="Q21" s="171">
         <v>0.1</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>55.657085344049747</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B22" s="38" t="s">
         <v>32</v>
       </c>
@@ -5119,7 +5119,7 @@
         <f>N20*N21</f>
         <v>31981353.756468486</v>
       </c>
-      <c r="P22" s="208"/>
+      <c r="P22" s="210"/>
       <c r="Q22" s="171">
         <v>0.105</v>
       </c>
@@ -5142,7 +5142,7 @@
         <v>51.831140321076028</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B23" s="38" t="s">
         <v>33</v>
       </c>
@@ -5168,7 +5168,7 @@
         <f>N16</f>
         <v>0.6793222995911935</v>
       </c>
-      <c r="P23" s="208"/>
+      <c r="P23" s="210"/>
       <c r="Q23" s="171">
         <v>0.11</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>48.552382738782562</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:40" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="73" t="s">
         <v>34</v>
       </c>
@@ -5214,7 +5214,7 @@
         <f>N22*N23</f>
         <v>21725646.777883627</v>
       </c>
-      <c r="P24" s="208"/>
+      <c r="P24" s="210"/>
       <c r="Q24" s="171">
         <v>0.115</v>
       </c>
@@ -5237,14 +5237,14 @@
         <v>45.711362065696093</v>
       </c>
     </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B25" s="38"/>
       <c r="D25" s="72"/>
       <c r="F25" s="38"/>
       <c r="I25" s="72"/>
       <c r="K25" s="38"/>
       <c r="N25" s="72"/>
-      <c r="P25" s="208"/>
+      <c r="P25" s="210"/>
       <c r="Q25" s="172">
         <v>0.12</v>
       </c>
@@ -5267,12 +5267,12 @@
         <v>43.225990707674406</v>
       </c>
     </row>
-    <row r="26" spans="2:40" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="205" t="s">
+    <row r="26" spans="2:40" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="207" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="206"/>
-      <c r="D26" s="207"/>
+      <c r="C26" s="208"/>
+      <c r="D26" s="209"/>
       <c r="E26" s="4"/>
       <c r="F26" s="38" t="s">
         <v>35</v>
@@ -5289,7 +5289,7 @@
         <v>21725646.777883627</v>
       </c>
     </row>
-    <row r="27" spans="2:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
         <v>37</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>4344764.3240570379</v>
       </c>
     </row>
-    <row r="28" spans="2:40" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:40" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="38" t="s">
         <v>15</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B29" s="38" t="s">
         <v>0</v>
       </c>
@@ -5367,7 +5367,7 @@
         <f>C29</f>
         <v>-2505000</v>
       </c>
-      <c r="P29" s="208" t="s">
+      <c r="P29" s="210" t="s">
         <v>34</v>
       </c>
       <c r="Q29" s="55">
@@ -5393,7 +5393,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B30" s="38"/>
       <c r="D30" s="72"/>
       <c r="F30" s="81" t="s">
@@ -5414,7 +5414,7 @@
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="P30" s="208"/>
+      <c r="P30" s="210"/>
       <c r="Q30" s="171">
         <v>0.1</v>
       </c>
@@ -5438,12 +5438,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="2:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="205" t="s">
+    <row r="31" spans="2:40" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="207" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="206"/>
-      <c r="D31" s="207"/>
+      <c r="C31" s="208"/>
+      <c r="D31" s="209"/>
       <c r="E31" s="4"/>
       <c r="F31" s="73" t="s">
         <v>42</v>
@@ -5459,7 +5459,7 @@
         <f>N28-N29</f>
         <v>28575411.101940665</v>
       </c>
-      <c r="P31" s="208"/>
+      <c r="P31" s="210"/>
       <c r="Q31" s="171">
         <v>0.105</v>
       </c>
@@ -5484,7 +5484,7 @@
       <c r="AK31" s="188"/>
       <c r="AL31" s="188"/>
     </row>
-    <row r="32" spans="2:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:40" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="38" t="s">
         <v>16</v>
       </c>
@@ -5506,7 +5506,7 @@
         <f>C6</f>
         <v>459000</v>
       </c>
-      <c r="P32" s="208"/>
+      <c r="P32" s="210"/>
       <c r="Q32" s="171">
         <v>0.11</v>
       </c>
@@ -5533,7 +5533,7 @@
       <c r="AM32" s="189"/>
       <c r="AN32" s="190"/>
     </row>
-    <row r="33" spans="2:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:40" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="38" t="s">
         <v>31</v>
       </c>
@@ -5559,7 +5559,7 @@
         <f>ROUND(N31/N32,0)</f>
         <v>62</v>
       </c>
-      <c r="P33" s="208"/>
+      <c r="P33" s="210"/>
       <c r="Q33" s="171">
         <v>0.115</v>
       </c>
@@ -5586,7 +5586,7 @@
       <c r="AM33" s="189"/>
       <c r="AN33" s="190"/>
     </row>
-    <row r="34" spans="2:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:40" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="81" t="s">
         <v>231</v>
       </c>
@@ -5612,7 +5612,7 @@
         <f>N33/$C$5-1</f>
         <v>-0.9005326317140474</v>
       </c>
-      <c r="P34" s="208"/>
+      <c r="P34" s="210"/>
       <c r="Q34" s="172">
         <v>0.12</v>
       </c>
@@ -5639,7 +5639,7 @@
       <c r="AM34" s="189"/>
       <c r="AN34" s="193"/>
     </row>
-    <row r="35" spans="2:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:40" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q35" s="64"/>
       <c r="R35" s="36"/>
       <c r="S35" s="36"/>
@@ -5652,48 +5652,48 @@
       <c r="AM35" s="189"/>
       <c r="AN35" s="193"/>
     </row>
-    <row r="36" spans="2:40" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:40" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AK36" s="194"/>
       <c r="AL36" s="195"/>
       <c r="AM36" s="195"/>
     </row>
-    <row r="38" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.25">
       <c r="G38" s="196"/>
     </row>
-    <row r="39" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:40" x14ac:dyDescent="0.25">
       <c r="C39" s="19"/>
     </row>
-    <row r="46" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:40" x14ac:dyDescent="0.25">
       <c r="D46" s="93"/>
     </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.25">
       <c r="D47" s="93"/>
     </row>
-    <row r="48" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:40" x14ac:dyDescent="0.25">
       <c r="D48" s="93"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="93"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="93"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="93"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="93"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="93"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="93"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="93"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="93"/>
     </row>
   </sheetData>
@@ -5741,52 +5741,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0C8DD0-6399-644F-BAA1-BF78766BA224}">
   <dimension ref="B1:P61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="13.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
-    <col min="6" max="8" width="13.33203125" style="116" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="116" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="130" customWidth="1"/>
-    <col min="11" max="14" width="13.33203125" style="116" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="2" width="13.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.296875" style="1" customWidth="1"/>
+    <col min="6" max="8" width="13.296875" style="116" customWidth="1"/>
+    <col min="9" max="9" width="14.69921875" style="116" customWidth="1"/>
+    <col min="10" max="10" width="13.296875" style="130" customWidth="1"/>
+    <col min="11" max="14" width="13.296875" style="116" customWidth="1"/>
+    <col min="15" max="15" width="12.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="1"/>
+    <col min="17" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F1" s="130"/>
     </row>
-    <row r="2" spans="2:16" s="109" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" s="109" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="107" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="108"/>
       <c r="D2" s="108"/>
       <c r="E2" s="108"/>
-      <c r="F2" s="213" t="s">
+      <c r="F2" s="215" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="214"/>
-      <c r="H2" s="214"/>
-      <c r="I2" s="215"/>
-      <c r="J2" s="213" t="s">
+      <c r="G2" s="216"/>
+      <c r="H2" s="216"/>
+      <c r="I2" s="217"/>
+      <c r="J2" s="215" t="s">
         <v>194</v>
       </c>
-      <c r="K2" s="214"/>
-      <c r="L2" s="214"/>
-      <c r="M2" s="214"/>
-      <c r="N2" s="214"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="K2" s="216"/>
+      <c r="L2" s="216"/>
+      <c r="M2" s="216"/>
+      <c r="N2" s="216"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>195</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>46</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>30458432.149017606</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="16" t="s">
         <v>47</v>
       </c>
@@ -5889,11 +5889,11 @@
         <f>H4/G4-1</f>
         <v>-0.99999650632442616</v>
       </c>
-      <c r="I5" s="212">
+      <c r="I5" s="214">
         <f>(I4+J4)/H4-1</f>
         <v>1946099</v>
       </c>
-      <c r="J5" s="212"/>
+      <c r="J5" s="214"/>
       <c r="K5" s="120">
         <v>0.11700000000000001</v>
       </c>
@@ -5907,11 +5907,11 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E6" s="116"/>
       <c r="P6" s="30"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
@@ -5954,13 +5954,13 @@
         <v>3563636.5614350601</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="123">
-        <f t="shared" ref="D8:E8" si="3">D7/D4</f>
+        <f t="shared" ref="D8" si="3">D7/D4</f>
         <v>0.65567527273995141</v>
       </c>
       <c r="E8" s="123">
@@ -5999,12 +5999,12 @@
         <v>0.11700000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="125">
-        <f t="shared" ref="D9:E9" si="5">D4-D7</f>
+        <f t="shared" ref="D9" si="5">D4-D7</f>
         <v>780172</v>
       </c>
       <c r="E9" s="125">
@@ -6048,12 +6048,12 @@
         <v>26894795.587582547</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="119">
-        <f t="shared" ref="D10:E10" si="7">D9/D4</f>
+        <f t="shared" ref="D10" si="7">D9/D4</f>
         <v>0.34432472726004865</v>
       </c>
       <c r="E10" s="119">
@@ -6097,7 +6097,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="15"/>
       <c r="D11" s="119"/>
       <c r="E11" s="119"/>
@@ -6111,24 +6111,24 @@
       <c r="M11" s="119"/>
       <c r="N11" s="119"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D12" s="219">
+      <c r="D12" s="198">
         <v>32048</v>
       </c>
-      <c r="E12" s="218">
+      <c r="E12" s="197">
         <v>18218</v>
       </c>
-      <c r="F12" s="218">
+      <c r="F12" s="197">
         <v>18218</v>
       </c>
-      <c r="G12" s="218">
+      <c r="G12" s="197">
         <v>19552</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>204</v>
       </c>
@@ -6171,13 +6171,13 @@
         <v>10569075.955709109</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="128">
-        <f t="shared" ref="D14:E14" si="10">D13/D4</f>
+        <f t="shared" ref="D14" si="10">D13/D4</f>
         <v>5.2134276457397224E-2</v>
       </c>
       <c r="E14" s="128">
@@ -6216,7 +6216,7 @@
         <v>0.34699999999999998</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>243</v>
       </c>
@@ -6259,33 +6259,33 @@
         <v>274125.88934115844</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="128">
-        <f>D15/D4</f>
+        <f t="shared" ref="D16:I16" si="12">D15/D4</f>
         <v>1.2152865893460287E-2</v>
       </c>
       <c r="E16" s="128">
-        <f>E15/E4</f>
+        <f t="shared" si="12"/>
         <v>1.4115159326114974E-2</v>
       </c>
       <c r="F16" s="128">
-        <f>F15/F4</f>
+        <f t="shared" si="12"/>
         <v>1.3374287103421131E-2</v>
       </c>
       <c r="G16" s="128">
-        <f>G15/G4</f>
+        <f t="shared" si="12"/>
         <v>2.2177153807320299E-2</v>
       </c>
       <c r="H16" s="128">
-        <f>H15/H4</f>
+        <f t="shared" si="12"/>
         <v>16900</v>
       </c>
       <c r="I16" s="128">
-        <f>I15/I4</f>
+        <f t="shared" si="12"/>
         <v>8.7737622728222275E-3</v>
       </c>
       <c r="J16" s="146">
@@ -6304,7 +6304,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>13</v>
       </c>
@@ -6321,89 +6321,89 @@
         <v>435095</v>
       </c>
       <c r="G17" s="125">
-        <f t="shared" ref="G17:N17" si="12">G9+G12-G13-G15</f>
+        <f t="shared" ref="G17:N17" si="13">G9+G12-G13-G15</f>
         <v>927288</v>
       </c>
       <c r="H17" s="125">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-8520990</v>
       </c>
       <c r="I17" s="125">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7491000</v>
       </c>
       <c r="J17" s="125">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2657100</v>
       </c>
       <c r="K17" s="125">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>11325465.176999999</v>
       </c>
       <c r="L17" s="125">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>12796232.256483003</v>
       </c>
       <c r="M17" s="125">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>14331780.127260963</v>
       </c>
       <c r="N17" s="125">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>16051593.742532279</v>
       </c>
       <c r="O17" s="30"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="129">
-        <f>D17/D4</f>
+        <f t="shared" ref="D18:N18" si="14">D17/D4</f>
         <v>0.29418179779972048</v>
       </c>
       <c r="E18" s="129">
-        <f>E17/E4</f>
+        <f t="shared" si="14"/>
         <v>0.22311315536965151</v>
       </c>
       <c r="F18" s="129">
-        <f>F17/F4</f>
+        <f t="shared" si="14"/>
         <v>0.22385402759234535</v>
       </c>
       <c r="G18" s="129">
-        <f>G17/G4</f>
+        <f t="shared" si="14"/>
         <v>0.32396434354709386</v>
       </c>
       <c r="H18" s="129">
-        <f>H17/H4</f>
+        <f t="shared" si="14"/>
         <v>-852099</v>
       </c>
       <c r="I18" s="129">
-        <f>I17/I4</f>
+        <f t="shared" si="14"/>
         <v>0.52162105702945483</v>
       </c>
       <c r="J18" s="129">
-        <f>J17/J4</f>
+        <f t="shared" si="14"/>
         <v>0.52100000000000002</v>
       </c>
       <c r="K18" s="129">
-        <f>K17/K4</f>
+        <f t="shared" si="14"/>
         <v>0.52100000000000002</v>
       </c>
       <c r="L18" s="129">
-        <f>L17/L4</f>
+        <f t="shared" si="14"/>
         <v>0.52700000000000014</v>
       </c>
       <c r="M18" s="129">
-        <f>M17/M4</f>
+        <f t="shared" si="14"/>
         <v>0.52700000000000002</v>
       </c>
       <c r="N18" s="129">
-        <f>N17/N4</f>
+        <f t="shared" si="14"/>
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>244</v>
       </c>
@@ -6420,7 +6420,7 @@
       <c r="N19" s="125"/>
       <c r="O19" s="30"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
         <v>245</v>
       </c>
@@ -6436,7 +6436,7 @@
       <c r="M20" s="141"/>
       <c r="N20" s="141"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="15"/>
       <c r="E21" s="129"/>
       <c r="F21" s="129"/>
@@ -6449,7 +6449,7 @@
       <c r="M21" s="129"/>
       <c r="N21" s="129"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>198</v>
       </c>
@@ -6492,33 +6492,33 @@
         <v>1522921.6074508803</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="17" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="128">
-        <f>D22/D4</f>
+        <f t="shared" ref="D23:I23" si="15">D22/D4</f>
         <v>8.9268131430667183E-2</v>
       </c>
       <c r="E23" s="128">
-        <f>E22/E4</f>
+        <f t="shared" si="15"/>
         <v>0.10491162269024081</v>
       </c>
       <c r="F23" s="128">
-        <f>F22/F4</f>
+        <f t="shared" si="15"/>
         <v>0.10491162269024081</v>
       </c>
       <c r="G23" s="128">
-        <f>G22/G4</f>
+        <f t="shared" si="15"/>
         <v>7.4848156125374044E-2</v>
       </c>
       <c r="H23" s="128">
-        <f>H22/H4</f>
+        <f t="shared" si="15"/>
         <v>85600</v>
       </c>
       <c r="I23" s="128">
-        <f>I22/I4</f>
+        <f t="shared" si="15"/>
         <v>4.5261472042336888E-2</v>
       </c>
       <c r="J23" s="146">
@@ -6537,101 +6537,101 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="125">
-        <f t="shared" ref="D24:N24" si="13">D19+D22</f>
+        <f t="shared" ref="D24:N24" si="16">D19+D22</f>
         <v>202264</v>
       </c>
       <c r="E24" s="125">
-        <f t="shared" ref="E24" si="14">E19+E22</f>
+        <f t="shared" ref="E24" si="17">E19+E22</f>
         <v>203912</v>
       </c>
       <c r="F24" s="125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>203912</v>
       </c>
       <c r="G24" s="125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>214239</v>
       </c>
       <c r="H24" s="125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>856000</v>
       </c>
       <c r="I24" s="125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>650000</v>
       </c>
       <c r="J24" s="125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>255000</v>
       </c>
       <c r="K24" s="125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1086896.8500000001</v>
       </c>
       <c r="L24" s="125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1214063.7814500001</v>
       </c>
       <c r="M24" s="125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1359751.4352240004</v>
       </c>
       <c r="N24" s="125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1522921.6074508803</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="143">
-        <f>E24/E4</f>
+        <f t="shared" ref="E25:N25" si="18">E24/E4</f>
         <v>0.10491162269024081</v>
       </c>
       <c r="F25" s="143">
-        <f>F24/F4</f>
+        <f t="shared" si="18"/>
         <v>0.10491162269024081</v>
       </c>
       <c r="G25" s="143">
-        <f>G24/G4</f>
+        <f t="shared" si="18"/>
         <v>7.4848156125374044E-2</v>
       </c>
       <c r="H25" s="143">
-        <f>H24/H4</f>
+        <f t="shared" si="18"/>
         <v>85600</v>
       </c>
       <c r="I25" s="143">
-        <f>I24/I4</f>
+        <f t="shared" si="18"/>
         <v>4.5261472042336888E-2</v>
       </c>
       <c r="J25" s="143">
-        <f>J24/J4</f>
+        <f t="shared" si="18"/>
         <v>0.05</v>
       </c>
       <c r="K25" s="143">
-        <f>K24/K4</f>
+        <f t="shared" si="18"/>
         <v>0.05</v>
       </c>
       <c r="L25" s="143">
-        <f>L24/L4</f>
+        <f t="shared" si="18"/>
         <v>0.05</v>
       </c>
       <c r="M25" s="143">
-        <f>M24/M4</f>
+        <f t="shared" si="18"/>
         <v>5.000000000000001E-2</v>
       </c>
       <c r="N25" s="143">
-        <f>N24/N4</f>
+        <f t="shared" si="18"/>
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="F26" s="143"/>
       <c r="G26" s="143"/>
@@ -6643,7 +6643,7 @@
       <c r="M26" s="143"/>
       <c r="N26" s="143"/>
     </row>
-    <row r="28" spans="2:15" s="109" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" s="109" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="107" t="s">
         <v>55</v>
       </c>
@@ -6660,7 +6660,7 @@
       <c r="M28" s="115"/>
       <c r="N28" s="115"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="13" t="s">
         <v>195</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>56</v>
       </c>
@@ -6714,7 +6714,7 @@
       <c r="M31" s="132"/>
       <c r="N31" s="132"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
         <v>49</v>
       </c>
@@ -6723,14 +6723,14 @@
       <c r="F32" s="129"/>
       <c r="G32" s="129"/>
       <c r="H32" s="129"/>
-      <c r="I32" s="209"/>
-      <c r="J32" s="210"/>
+      <c r="I32" s="211"/>
+      <c r="J32" s="212"/>
       <c r="K32" s="133"/>
       <c r="L32" s="133"/>
       <c r="M32" s="133"/>
       <c r="N32" s="133"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>57</v>
       </c>
@@ -6746,7 +6746,7 @@
       <c r="M33" s="126"/>
       <c r="N33" s="126"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
         <v>49</v>
       </c>
@@ -6755,14 +6755,14 @@
       <c r="F34" s="129"/>
       <c r="G34" s="129"/>
       <c r="H34" s="129"/>
-      <c r="I34" s="209"/>
-      <c r="J34" s="210"/>
+      <c r="I34" s="211"/>
+      <c r="J34" s="212"/>
       <c r="K34" s="133"/>
       <c r="L34" s="133"/>
       <c r="M34" s="133"/>
       <c r="N34" s="133"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>58</v>
       </c>
@@ -6778,7 +6778,7 @@
       <c r="M35" s="132"/>
       <c r="N35" s="132"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="17" t="s">
         <v>49</v>
       </c>
@@ -6788,14 +6788,14 @@
       <c r="F36" s="128"/>
       <c r="G36" s="128"/>
       <c r="H36" s="128"/>
-      <c r="I36" s="211"/>
-      <c r="J36" s="216"/>
+      <c r="I36" s="213"/>
+      <c r="J36" s="218"/>
       <c r="K36" s="134"/>
       <c r="L36" s="134"/>
       <c r="M36" s="134"/>
       <c r="N36" s="134"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>59</v>
       </c>
@@ -6811,7 +6811,7 @@
       <c r="M37" s="127"/>
       <c r="N37" s="127"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>180</v>
       </c>
@@ -6827,7 +6827,7 @@
       <c r="M39" s="132"/>
       <c r="N39" s="132"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="s">
         <v>49</v>
       </c>
@@ -6836,14 +6836,14 @@
       <c r="F40" s="129"/>
       <c r="G40" s="129"/>
       <c r="H40" s="129"/>
-      <c r="I40" s="209"/>
-      <c r="J40" s="210"/>
+      <c r="I40" s="211"/>
+      <c r="J40" s="212"/>
       <c r="K40" s="133"/>
       <c r="L40" s="133"/>
       <c r="M40" s="133"/>
       <c r="N40" s="133"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>197</v>
       </c>
@@ -6859,7 +6859,7 @@
       <c r="M41" s="132"/>
       <c r="N41" s="132"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="s">
         <v>49</v>
       </c>
@@ -6868,14 +6868,14 @@
       <c r="F42" s="129"/>
       <c r="G42" s="129"/>
       <c r="H42" s="129"/>
-      <c r="I42" s="211"/>
-      <c r="J42" s="211"/>
+      <c r="I42" s="213"/>
+      <c r="J42" s="213"/>
       <c r="K42" s="140"/>
       <c r="L42" s="140"/>
       <c r="M42" s="140"/>
       <c r="N42" s="140"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="37" t="s">
         <v>60</v>
       </c>
@@ -6892,7 +6892,7 @@
       <c r="M43" s="135"/>
       <c r="N43" s="135"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>59</v>
       </c>
@@ -6908,7 +6908,7 @@
       <c r="M45" s="127"/>
       <c r="N45" s="127"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
         <v>60</v>
       </c>
@@ -6925,7 +6925,7 @@
       <c r="M46" s="136"/>
       <c r="N46" s="136"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>61</v>
       </c>
@@ -6941,7 +6941,7 @@
       <c r="M47" s="127"/>
       <c r="N47" s="127"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
         <v>62</v>
       </c>
@@ -6957,7 +6957,7 @@
       <c r="M48" s="125"/>
       <c r="N48" s="125"/>
     </row>
-    <row r="50" spans="2:14" s="109" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:14" s="109" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="107" t="s">
         <v>192</v>
       </c>
@@ -6974,7 +6974,7 @@
       <c r="M50" s="115"/>
       <c r="N50" s="115"/>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" s="13" t="s">
         <v>195</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
         <v>63</v>
       </c>
@@ -7028,7 +7028,7 @@
       <c r="M53" s="138"/>
       <c r="N53" s="138"/>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B54" s="15" t="s">
         <v>49</v>
       </c>
@@ -7044,11 +7044,11 @@
       <c r="M54" s="142"/>
       <c r="N54" s="142"/>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H55" s="139"/>
       <c r="I55" s="139"/>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:14" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B57" s="107" t="s">
         <v>242</v>
       </c>
@@ -7065,7 +7065,7 @@
       <c r="M57" s="115"/>
       <c r="N57" s="115"/>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B58" s="13" t="s">
         <v>195</v>
       </c>
@@ -7103,7 +7103,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
         <v>242</v>
       </c>
@@ -7119,7 +7119,7 @@
       <c r="M60" s="138"/>
       <c r="N60" s="138"/>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B61" s="15" t="s">
         <v>49</v>
       </c>
@@ -7155,28 +7155,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F4C05E-7F42-DB47-862E-0113684357CE}">
   <dimension ref="C6:F9"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="84" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="179"/>
-    <col min="3" max="3" width="10.1640625" style="179" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="179"/>
-    <col min="5" max="6" width="13.6640625" style="179" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="179"/>
+    <col min="1" max="2" width="10.796875" style="179"/>
+    <col min="3" max="3" width="10.19921875" style="179" customWidth="1"/>
+    <col min="4" max="4" width="10.796875" style="179"/>
+    <col min="5" max="6" width="13.69921875" style="179" customWidth="1"/>
+    <col min="7" max="16384" width="10.796875" style="179"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="217" t="s">
+    <row r="6" spans="3:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="219" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="217"/>
-      <c r="E6" s="217"/>
-      <c r="F6" s="217"/>
-    </row>
-    <row r="7" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="219"/>
+      <c r="E6" s="219"/>
+      <c r="F6" s="219"/>
+    </row>
+    <row r="7" spans="3:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="180"/>
       <c r="D7" s="181" t="s">
         <v>224</v>
@@ -7188,7 +7188,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="181" t="s">
         <v>226</v>
       </c>
@@ -7196,7 +7196,7 @@
       <c r="E8" s="180"/>
       <c r="F8" s="180"/>
     </row>
-    <row r="9" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="181" t="s">
         <v>2</v>
       </c>
@@ -7221,45 +7221,45 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.83203125" customWidth="1"/>
+    <col min="1" max="1" width="45.796875" customWidth="1"/>
     <col min="2" max="5" width="11" customWidth="1"/>
-    <col min="6" max="8" width="10.83203125" customWidth="1"/>
+    <col min="6" max="8" width="10.796875" customWidth="1"/>
     <col min="9" max="196" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>69</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>74</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>75</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>77</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>178</v>
       </c>
@@ -7379,7 +7379,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>79</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>3764</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>80</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>81</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>82</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>83</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>-46</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>84</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>85</v>
       </c>
@@ -7547,7 +7547,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>186</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>87</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>2211</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>88</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>89</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>90</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>91</v>
       </c>
@@ -7691,7 +7691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>92</v>
       </c>
@@ -7715,7 +7715,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>93</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>8889</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>94</v>
       </c>
@@ -7763,7 +7763,7 @@
         <v>20308</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>95</v>
       </c>
@@ -7787,7 +7787,7 @@
         <v>-6741</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>96</v>
       </c>
@@ -7811,7 +7811,7 @@
         <v>13567</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
         <v>97</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>3831</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>98</v>
       </c>
@@ -7859,7 +7859,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
         <v>99</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>7422</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
         <v>100</v>
       </c>
@@ -7907,7 +7907,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>181</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
         <v>187</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>101</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="24" t="s">
         <v>102</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>35439</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="24" t="s">
         <v>103</v>
       </c>
@@ -8027,7 +8027,7 @@
         <v>3217</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>104</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
         <v>105</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="24" t="s">
         <v>106</v>
       </c>
@@ -8099,7 +8099,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>107</v>
       </c>
@@ -8123,7 +8123,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
         <v>108</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v>4985</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="24" t="s">
         <v>109</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="24" t="s">
         <v>110</v>
       </c>
@@ -8195,7 +8195,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="24" t="s">
         <v>111</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="24" t="s">
         <v>112</v>
       </c>
@@ -8243,7 +8243,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="24" t="s">
         <v>110</v>
       </c>
@@ -8267,7 +8267,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="24" t="s">
         <v>113</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="24" t="s">
         <v>114</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
         <v>115</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>7426</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
         <v>116</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>4996</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="24" t="s">
         <v>118</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>1646</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="24" t="s">
         <v>119</v>
       </c>
@@ -8411,7 +8411,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="24" t="s">
         <v>120</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="24" t="s">
         <v>117</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="24" t="s">
         <v>121</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="24" t="s">
         <v>122</v>
       </c>
@@ -8507,7 +8507,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="24" t="s">
         <v>123</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
         <v>124</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="24" t="s">
         <v>113</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>-1382</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="24" t="s">
         <v>125</v>
       </c>
@@ -8603,7 +8603,7 @@
         <v>6593</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="24" t="s">
         <v>126</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>3486</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="24" t="s">
         <v>127</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="24" t="s">
         <v>128</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
         <v>129</v>
       </c>
@@ -8699,7 +8699,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="24" t="s">
         <v>112</v>
       </c>
@@ -8723,7 +8723,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="24" t="s">
         <v>130</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="24" t="s">
         <v>101</v>
       </c>
@@ -8772,7 +8772,7 @@
       </c>
       <c r="K75" s="25"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
         <v>131</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>20236</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="24" t="s">
         <v>132</v>
       </c>
@@ -8821,7 +8821,7 @@
       </c>
       <c r="K77" s="25"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
         <v>133</v>
       </c>
@@ -8845,7 +8845,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="24" t="s">
         <v>134</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>14999</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="24" t="s">
         <v>135</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>-663</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
         <v>136</v>
       </c>
@@ -8917,7 +8917,7 @@
         <v>15203</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
         <v>137</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
         <v>138</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>15203</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="24" t="s">
         <v>139</v>
       </c>
@@ -9005,32 +9005,32 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.83203125" customWidth="1"/>
+    <col min="1" max="1" width="45.796875" customWidth="1"/>
     <col min="2" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" customWidth="1"/>
     <col min="8" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" customWidth="1"/>
+    <col min="12" max="12" width="18.796875" customWidth="1"/>
     <col min="13" max="190" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="48" t="s">
         <v>67</v>
       </c>
@@ -9040,7 +9040,7 @@
       <c r="E9" s="49"/>
       <c r="F9" s="49"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="47" t="s">
         <v>175</v>
       </c>
@@ -9050,7 +9050,7 @@
       <c r="E12" s="49"/>
       <c r="F12" s="49"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
         <v>69</v>
       </c>
@@ -9070,7 +9070,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="46" t="s">
         <v>74</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="46" t="s">
         <v>75</v>
       </c>
@@ -9110,7 +9110,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="46" t="s">
         <v>77</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="46" t="s">
         <v>178</v>
       </c>
@@ -9150,7 +9150,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="44" t="s">
         <v>174</v>
       </c>
@@ -9170,7 +9170,7 @@
         <v>57113</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="44" t="s">
         <v>173</v>
       </c>
@@ -9190,7 +9190,7 @@
         <v>-44488</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="44" t="s">
         <v>172</v>
       </c>
@@ -9210,7 +9210,7 @@
         <v>12625</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="44" t="s">
         <v>171</v>
       </c>
@@ -9230,7 +9230,7 @@
         <v>-6426</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="44" t="s">
         <v>170</v>
       </c>
@@ -9250,7 +9250,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="44" t="s">
         <v>169</v>
       </c>
@@ -9270,7 +9270,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="44" t="s">
         <v>188</v>
       </c>
@@ -9290,7 +9290,7 @@
         <v>-1696</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="44" t="s">
         <v>168</v>
       </c>
@@ -9310,7 +9310,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="44" t="s">
         <v>167</v>
       </c>
@@ -9330,7 +9330,7 @@
         <v>-8037</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="44" t="s">
         <v>166</v>
       </c>
@@ -9350,7 +9350,7 @@
         <v>4588</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="44" t="s">
         <v>165</v>
       </c>
@@ -9370,7 +9370,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="44" t="s">
         <v>164</v>
       </c>
@@ -9390,7 +9390,7 @@
         <v>-266</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="44" t="s">
         <v>163</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>-110</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="44" t="s">
         <v>189</v>
       </c>
@@ -9430,7 +9430,7 @@
         <v>-36</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="44" t="s">
         <v>162</v>
       </c>
@@ -9450,7 +9450,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="44" t="s">
         <v>161</v>
       </c>
@@ -9470,7 +9470,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="44" t="s">
         <v>160</v>
       </c>
@@ -9490,7 +9490,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="44" t="s">
         <v>159</v>
       </c>
@@ -9510,7 +9510,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="44" t="s">
         <v>158</v>
       </c>
@@ -9530,7 +9530,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="44" t="s">
         <v>157</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>-446</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="44" t="s">
         <v>156</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="44" t="s">
         <v>155</v>
       </c>
@@ -9590,7 +9590,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="44" t="s">
         <v>154</v>
       </c>
@@ -9610,7 +9610,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="44" t="s">
         <v>153</v>
       </c>
@@ -9630,7 +9630,7 @@
         <v>-56</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="44" t="s">
         <v>152</v>
       </c>
@@ -9650,7 +9650,7 @@
         <v>-427</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="44" t="s">
         <v>151</v>
       </c>
@@ -9670,7 +9670,7 @@
         <v>4193</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="44" t="s">
         <v>150</v>
       </c>
@@ -9690,7 +9690,7 @@
         <v>-816</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="44" t="s">
         <v>149</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>3377</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="44" t="s">
         <v>148</v>
       </c>
@@ -9730,7 +9730,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="44" t="s">
         <v>147</v>
       </c>
@@ -9750,7 +9750,7 @@
         <v>3377</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="44" t="s">
         <v>146</v>
       </c>
@@ -9770,7 +9770,7 @@
         <v>1105.3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="44" t="s">
         <v>145</v>
       </c>
@@ -9790,7 +9790,7 @@
         <v>1106.7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="44" t="s">
         <v>144</v>
       </c>
@@ -9810,7 +9810,7 @@
         <v>1079.6120000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="44" t="s">
         <v>143</v>
       </c>
@@ -9830,7 +9830,7 @@
         <v>3.0579999999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="44" t="s">
         <v>142</v>
       </c>
@@ -9850,7 +9850,7 @@
         <v>3.0449999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="44" t="s">
         <v>141</v>
       </c>
@@ -9870,7 +9870,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="44" t="s">
         <v>140</v>
       </c>

</xml_diff>